<commit_message>
move parser to class
</commit_message>
<xml_diff>
--- a/excel/output.xlsx
+++ b/excel/output.xlsx
@@ -1230,6 +1230,254 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="1.a Screenshots_E3.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7962900" y="381000"/>
+          <a:ext cx="18268950" cy="10287000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="1.a Screenshots_E15.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7962900" y="5029200"/>
+          <a:ext cx="16478250" cy="10601325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="2 User Access Review_D1.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6143625" y="0"/>
+          <a:ext cx="23812500" cy="15630525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="3.a Screenshots_E3.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8020050" y="381000"/>
+          <a:ext cx="23812500" cy="15506700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="3.a Screenshots_E15.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8020050" y="5829300"/>
+          <a:ext cx="23812500" cy="15363825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="4 Post Review_D1.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6143625" y="0"/>
+          <a:ext cx="23812500" cy="15630525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1771,6 +2019,7 @@
     <row r="62" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4763,6 +5012,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5025,6 +5275,7 @@
     <row r="34" ht="13" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7896,5 +8147,6 @@
     <row r="24" spans="2:5" ht="13" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
reformat helpers & pseudocode
</commit_message>
<xml_diff>
--- a/excel/output.xlsx
+++ b/excel/output.xlsx
@@ -1230,254 +1230,6 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="1.a Screenshots_E3.jpg"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7962900" y="381000"/>
-          <a:ext cx="18268950" cy="10287000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="1.a Screenshots_E15.jpg"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7962900" y="5029200"/>
-          <a:ext cx="16478250" cy="10601325"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="2 User Access Review_D1.jpg"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6143625" y="0"/>
-          <a:ext cx="23812500" cy="15630525"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>43</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="3.a Screenshots_E3.jpg"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8020050" y="381000"/>
-          <a:ext cx="23812500" cy="15506700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>43</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>87</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="3.a Screenshots_E15.jpg"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8020050" y="5829300"/>
-          <a:ext cx="23812500" cy="15363825"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>40</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="4 Post Review_D1.jpg"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6143625" y="0"/>
-          <a:ext cx="23812500" cy="15630525"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2019,7 +1771,6 @@
     <row r="62" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5012,7 +4763,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5275,7 +5025,6 @@
     <row r="34" ht="13" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8147,6 +7896,5 @@
     <row r="24" spans="2:5" ht="13" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add sheet rels & tag
</commit_message>
<xml_diff>
--- a/excel/output.xlsx
+++ b/excel/output.xlsx
@@ -1232,7 +1232,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="UTF-8" standalone="yes"?><xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"><xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:ns3="http://schemas.openxmlformats.org/officeDocument/2006/relationships"><xdr:from><xdr:col>4</xdr:col><xdr:colOff>0</xdr:colOff><xdr:row>14</xdr:row><xdr:rowOff>0</xdr:rowOff></xdr:from><xdr:ext cx="9194800" cy="5372100" /><xdr:pic><xdr:nvPicPr><xdr:cNvPr id="8" name="image2.png"><a:extLst><a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}"><a16:creationId id="{00000000-0008-0000-0100-000008000000}" /></a:ext></a:extLst></xdr:cNvPr><xdr:cNvPicPr preferRelativeResize="0" /></xdr:nvPicPr><xdr:blipFill><a:blip ns3:embed="rId1" cstate="print" /><a:stretch><a:fillRect /></a:stretch></xdr:blipFill><xdr:spPr><a:xfrm><a:off x="9207500" y="5041900" /><a:ext cx="9194800" cy="5372100" /></a:xfrm><a:prstGeom prst="rect"><a:avLst /></a:prstGeom><a:noFill /></xdr:spPr></xdr:pic><xdr:clientData fLocksWithSheet="0" /></xdr:oneCellAnchor><xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main"><xdr:from><xdr:col>11</xdr:col><xdr:colOff>180975</xdr:colOff><xdr:row>29</xdr:row><xdr:rowOff>95250</xdr:rowOff></xdr:from><xdr:ext cx="676275" cy="190500" /><xdr:sp macro="" textlink=""><xdr:nvSpPr><xdr:cNvPr id="3" name="Shape 3"><a:extLst><a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}"><a16:creationId id="{00000000-0008-0000-0100-000003000000}" /></a:ext></a:extLst></xdr:cNvPr><xdr:cNvSpPr /></xdr:nvSpPr><xdr:spPr><a:xfrm><a:off x="16144875" y="9950450" /><a:ext cx="676275" cy="190500" /></a:xfrm><a:prstGeom prst="rect"><a:avLst /></a:prstGeom><a:noFill /><a:ln w="76200" cap="flat" cmpd="sng"><a:solidFill><a:srgbClr val="FF0000" /></a:solidFill><a:prstDash val="solid" /><a:round /><a:headEnd type="none" w="sm" len="sm" /><a:tailEnd type="none" w="sm" len="sm" /></a:ln></xdr:spPr><xdr:txBody><a:bodyPr spcFirstLastPara="1" wrap="square" lIns="91425" tIns="91425" rIns="91425" bIns="91425" anchor="ctr" anchorCtr="0"><a:noAutofit /></a:bodyPr><a:lstStyle /><a:p><a:pPr marL="0" lvl="0" indent="0" algn="ctr" rtl="0"><a:spcBef><a:spcPts val="0" /></a:spcBef><a:spcAft><a:spcPts val="0" /></a:spcAft><a:buNone /></a:pPr><a:endParaRPr sz="1400" /></a:p></xdr:txBody></xdr:sp><xdr:clientData fLocksWithSheet="0" /></xdr:oneCellAnchor><xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main"><xdr:from><xdr:col>4</xdr:col><xdr:colOff>47625</xdr:colOff><xdr:row>25</xdr:row><xdr:rowOff>92074</xdr:rowOff></xdr:from><xdr:ext cx="6734175" cy="796925" /><xdr:grpSp><xdr:nvGrpSpPr><xdr:cNvPr id="2" name="Shape 2" title="Drawing"><a:extLst><a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}"><a16:creationId id="{00000000-0008-0000-0100-000002000000}" /></a:ext></a:extLst></xdr:cNvPr><xdr:cNvGrpSpPr /></xdr:nvGrpSpPr><xdr:grpSpPr><a:xfrm><a:off x="9255125" y="9159874" /><a:ext cx="6734175" cy="796925" /><a:chOff x="2243550" y="4293375" /><a:chExt cx="6030300" cy="89700" /></a:xfrm></xdr:grpSpPr><xdr:cxnSp macro=""><xdr:nvCxnSpPr><xdr:cNvPr id="4" name="Shape 4"><a:extLst><a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}"><a16:creationId id="{00000000-0008-0000-0100-000004000000}" /></a:ext></a:extLst></xdr:cNvPr><xdr:cNvCxnSpPr /></xdr:nvCxnSpPr><xdr:spPr><a:xfrm rot="10800000"><a:off x="2243550" y="4293375" /><a:ext cx="6030300" cy="89700" /></a:xfrm><a:prstGeom prst="straightConnector1"><a:avLst /></a:prstGeom><a:noFill /><a:ln w="28575" cap="flat" cmpd="sng"><a:solidFill><a:srgbClr val="FF0000" /></a:solidFill><a:prstDash val="solid" /><a:round /><a:headEnd type="none" w="med" len="med" /><a:tailEnd type="triangle" w="med" len="med" /></a:ln></xdr:spPr></xdr:cxnSp></xdr:grpSp><xdr:clientData fLocksWithSheet="0" /></xdr:oneCellAnchor><xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main"><xdr:from><xdr:col>0</xdr:col><xdr:colOff>2657475</xdr:colOff><xdr:row>16</xdr:row><xdr:rowOff>200025</xdr:rowOff></xdr:from><xdr:ext cx="2143125" cy="3181350" /><xdr:grpSp><xdr:nvGrpSpPr><xdr:cNvPr id="5" name="Shape 2" title="Drawing"><a:extLst><a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}"><a16:creationId id="{00000000-0008-0000-0100-000005000000}" /></a:ext></a:extLst></xdr:cNvPr><xdr:cNvGrpSpPr /></xdr:nvGrpSpPr><xdr:grpSpPr><a:xfrm><a:off x="2657475" y="5559425" /><a:ext cx="2143125" cy="3181350" /><a:chOff x="3052075" y="2001475" /><a:chExt cx="1841400" cy="2751900" /></a:xfrm></xdr:grpSpPr><xdr:cxnSp macro=""><xdr:nvCxnSpPr><xdr:cNvPr id="6" name="Shape 5"><a:extLst><a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}"><a16:creationId id="{00000000-0008-0000-0100-000006000000}" /></a:ext></a:extLst></xdr:cNvPr><xdr:cNvCxnSpPr /></xdr:nvCxnSpPr><xdr:spPr><a:xfrm rot="10800000"><a:off x="3052075" y="2001475" /><a:ext cx="1841400" cy="2751900" /></a:xfrm><a:prstGeom prst="straightConnector1"><a:avLst /></a:prstGeom><a:noFill /><a:ln w="28575" cap="flat" cmpd="sng"><a:solidFill><a:srgbClr val="FF0000" /></a:solidFill><a:prstDash val="solid" /><a:round /><a:headEnd type="none" w="med" len="med" /><a:tailEnd type="triangle" w="med" len="med" /></a:ln></xdr:spPr></xdr:cxnSp></xdr:grpSp><xdr:clientData fLocksWithSheet="0" /></xdr:oneCellAnchor><xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:ns3="http://schemas.openxmlformats.org/officeDocument/2006/relationships"><xdr:from><xdr:col>4</xdr:col><xdr:colOff>0</xdr:colOff><xdr:row>2</xdr:row><xdr:rowOff>0</xdr:rowOff></xdr:from><xdr:ext cx="8102600" cy="4292600" /><xdr:pic><xdr:nvPicPr><xdr:cNvPr id="7" name="image1.jpg"><a:extLst><a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}"><a16:creationId id="{00000000-0008-0000-0100-000007000000}" /></a:ext></a:extLst></xdr:cNvPr><xdr:cNvPicPr preferRelativeResize="0" /></xdr:nvPicPr><xdr:blipFill><a:blip ns3:embed="rId2" cstate="print" /><a:stretch><a:fillRect /></a:stretch></xdr:blipFill><xdr:spPr><a:xfrm><a:off x="9207500" y="381000" /><a:ext cx="8102600" cy="4292600" /></a:xfrm><a:prstGeom prst="rect"><a:avLst /></a:prstGeom><a:noFill /></xdr:spPr></xdr:pic><xdr:clientData fLocksWithSheet="0" /></xdr:oneCellAnchor></xdr:wsDr>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="UTF-8" standalone="yes"?><xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"><xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main"><xdr:from><xdr:col>11</xdr:col><xdr:colOff>180975</xdr:colOff><xdr:row>29</xdr:row><xdr:rowOff>95250</xdr:rowOff></xdr:from><xdr:ext cx="676275" cy="190500" /><xdr:sp macro="" textlink=""><xdr:nvSpPr><xdr:cNvPr id="3" name="Shape 3"><a:extLst><a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}"><a16:creationId id="{00000000-0008-0000-0100-000003000000}" /></a:ext></a:extLst></xdr:cNvPr><xdr:cNvSpPr /></xdr:nvSpPr><xdr:spPr><a:xfrm><a:off x="16144875" y="9950450" /><a:ext cx="676275" cy="190500" /></a:xfrm><a:prstGeom prst="rect"><a:avLst /></a:prstGeom><a:noFill /><a:ln w="76200" cap="flat" cmpd="sng"><a:solidFill><a:srgbClr val="FF0000" /></a:solidFill><a:prstDash val="solid" /><a:round /><a:headEnd type="none" w="sm" len="sm" /><a:tailEnd type="none" w="sm" len="sm" /></a:ln></xdr:spPr><xdr:txBody><a:bodyPr spcFirstLastPara="1" wrap="square" lIns="91425" tIns="91425" rIns="91425" bIns="91425" anchor="ctr" anchorCtr="0"><a:noAutofit /></a:bodyPr><a:lstStyle /><a:p><a:pPr marL="0" lvl="0" indent="0" algn="ctr" rtl="0"><a:spcBef><a:spcPts val="0" /></a:spcBef><a:spcAft><a:spcPts val="0" /></a:spcAft><a:buNone /></a:pPr><a:endParaRPr sz="1400" /></a:p></xdr:txBody></xdr:sp><xdr:clientData fLocksWithSheet="0" /></xdr:oneCellAnchor><xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main"><xdr:from><xdr:col>4</xdr:col><xdr:colOff>47625</xdr:colOff><xdr:row>25</xdr:row><xdr:rowOff>92074</xdr:rowOff></xdr:from><xdr:ext cx="6734175" cy="796925" /><xdr:grpSp><xdr:nvGrpSpPr><xdr:cNvPr id="2" name="Shape 2" title="Drawing"><a:extLst><a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}"><a16:creationId id="{00000000-0008-0000-0100-000002000000}" /></a:ext></a:extLst></xdr:cNvPr><xdr:cNvGrpSpPr /></xdr:nvGrpSpPr><xdr:grpSpPr><a:xfrm><a:off x="9266331" y="9221133" /><a:ext cx="6734175" cy="796925" /><a:chOff x="2243550" y="4293375" /><a:chExt cx="6030300" cy="89700" /></a:xfrm></xdr:grpSpPr><xdr:cxnSp macro=""><xdr:nvCxnSpPr><xdr:cNvPr id="4" name="Shape 4"><a:extLst><a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}"><a16:creationId id="{00000000-0008-0000-0100-000004000000}" /></a:ext></a:extLst></xdr:cNvPr><xdr:cNvCxnSpPr /></xdr:nvCxnSpPr><xdr:spPr><a:xfrm rot="10800000"><a:off x="2243550" y="4293375" /><a:ext cx="6030300" cy="89700" /></a:xfrm><a:prstGeom prst="straightConnector1"><a:avLst /></a:prstGeom><a:noFill /><a:ln w="28575" cap="flat" cmpd="sng"><a:solidFill><a:srgbClr val="FF0000" /></a:solidFill><a:prstDash val="solid" /><a:round /><a:headEnd type="none" w="med" len="med" /><a:tailEnd type="triangle" w="med" len="med" /></a:ln></xdr:spPr></xdr:cxnSp></xdr:grpSp><xdr:clientData fLocksWithSheet="0" /></xdr:oneCellAnchor><xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main"><xdr:from><xdr:col>0</xdr:col><xdr:colOff>2657475</xdr:colOff><xdr:row>16</xdr:row><xdr:rowOff>200025</xdr:rowOff></xdr:from><xdr:ext cx="2143125" cy="3181350" /><xdr:grpSp><xdr:nvGrpSpPr><xdr:cNvPr id="5" name="Shape 2" title="Drawing"><a:extLst><a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}"><a16:creationId id="{00000000-0008-0000-0100-000005000000}" /></a:ext></a:extLst></xdr:cNvPr><xdr:cNvGrpSpPr /></xdr:nvGrpSpPr><xdr:grpSpPr><a:xfrm><a:off x="2657475" y="5581090" /><a:ext cx="2143125" cy="3181350" /><a:chOff x="3052075" y="2001475" /><a:chExt cx="1841400" cy="2751900" /></a:xfrm></xdr:grpSpPr><xdr:cxnSp macro=""><xdr:nvCxnSpPr><xdr:cNvPr id="6" name="Shape 5"><a:extLst><a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}"><a16:creationId id="{00000000-0008-0000-0100-000006000000}" /></a:ext></a:extLst></xdr:cNvPr><xdr:cNvCxnSpPr /></xdr:nvCxnSpPr><xdr:spPr><a:xfrm rot="10800000"><a:off x="3052075" y="2001475" /><a:ext cx="1841400" cy="2751900" /></a:xfrm><a:prstGeom prst="straightConnector1"><a:avLst /></a:prstGeom><a:noFill /><a:ln w="28575" cap="flat" cmpd="sng"><a:solidFill><a:srgbClr val="FF0000" /></a:solidFill><a:prstDash val="solid" /><a:round /><a:headEnd type="none" w="med" len="med" /><a:tailEnd type="triangle" w="med" len="med" /></a:ln></xdr:spPr></xdr:cxnSp></xdr:grpSp><xdr:clientData fLocksWithSheet="0" /></xdr:oneCellAnchor></xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="UTF-8" standalone="yes"?><xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"><xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:ns3="http://schemas.openxmlformats.org/officeDocument/2006/relationships"><xdr:from><xdr:col>3</xdr:col><xdr:colOff>0</xdr:colOff><xdr:row>0</xdr:row><xdr:rowOff>0</xdr:rowOff></xdr:from><xdr:ext cx="295275" cy="200025" /><xdr:pic><xdr:nvPicPr><xdr:cNvPr id="2" name="image4.jpg"><a:extLst><a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}"><a16:creationId id="{00000000-0008-0000-0300-000002000000}" /></a:ext></a:extLst></xdr:cNvPr><xdr:cNvPicPr preferRelativeResize="0" /></xdr:nvPicPr><xdr:blipFill><a:blip ns3:embed="rId1" cstate="print" /><a:stretch><a:fillRect /></a:stretch></xdr:blipFill><xdr:spPr><a:prstGeom prst="rect"><a:avLst /></a:prstGeom><a:noFill /></xdr:spPr></xdr:pic><xdr:clientData fLocksWithSheet="0" /></xdr:oneCellAnchor></xdr:wsDr>
@@ -1682,108 +1682,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:N62"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="40.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="59" customWidth="1"/>
-    <col min="13" max="13" width="6.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:14" ht="13" customHeight="1">
-      <c r="N3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="13" customHeight="1"/>
-    <row r="5" spans="1:14" ht="13" customHeight="1"/>
-    <row r="6" spans="1:14" ht="13" customHeight="1">
-      <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="13" customHeight="1"/>
-    <row r="8" spans="1:14" ht="50.25" customHeight="1">
-      <c r="A8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="45" customHeight="1">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14"/>
-    <row r="11" spans="1:14"/>
-    <row r="12" spans="1:14" ht="147" customHeight="1"/>
-    <row r="13" spans="1:14">
-      <c r="K13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14"/>
-    <row r="15" spans="1:14" ht="13" customHeight="1">
-      <c r="A15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="13" customHeight="1"/>
-    <row r="17" spans="1:7">
-      <c r="A17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7"/>
-    <row r="19" spans="1:7"/>
-    <row r="20" spans="1:7"/>
-    <row r="21" spans="1:7" ht="169.5" customHeight="1"/>
-    <row r="22" spans="1:7"/>
-    <row r="23" spans="1:7"/>
-    <row r="24" spans="1:7" ht="16" customHeight="1">
-      <c r="C24" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="16" customHeight="1"/>
-    <row r="26" spans="1:7"/>
-    <row r="27" spans="1:7"/>
-    <row r="28" spans="1:7" ht="16" customHeight="1"/>
-    <row r="29" spans="1:7" ht="16" customHeight="1">
-      <c r="G29" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="16" customHeight="1"/>
-    <row r="31" spans="1:7" ht="13" customHeight="1"/>
-    <row r="49" ht="15.75" customHeight="1"/>
-    <row r="50" ht="15.75" customHeight="1"/>
-    <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
-    <row r="57" ht="15.75" customHeight="1"/>
-    <row r="58" ht="15.75" customHeight="1"/>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="15.75" customHeight="1"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<file path=xl/worksheets/sheet2.xml><?xml version='1.0' encoding='UTF-8'?>
+<worksheet><dimension ref="A3:N62" /><sheetViews><sheetView workbookViewId="0" /></sheetViews><sheetFormatPr defaultRowHeight="15" /><cols><col min="1" max="1" width="40.42578125" customWidth="1" /><col min="2" max="2" width="10.85546875" customWidth="1" /><col min="3" max="3" width="59" customWidth="1" /><col min="13" max="13" width="6.42578125" customWidth="1" /></cols><sheetData><row r="3" spans="1:14" ht="13" customHeight="1"><c r="N3" t="s"><v>29</v></c></row><row r="4" spans="1:14" ht="13" customHeight="1" /><row r="5" spans="1:14" ht="13" customHeight="1" /><row r="6" spans="1:14" ht="13" customHeight="1"><c r="A6" t="s"><v>30</v></c><c r="B6" t="s"><v>31</v></c></row><row r="7" spans="1:14" ht="13" customHeight="1" /><row r="8" spans="1:14" ht="50.25" customHeight="1"><c r="A8" t="s"><v>32</v></c></row><row r="9" spans="1:14" ht="45" customHeight="1"><c r="A9" t="s"><v>33</v></c></row><row r="10" spans="1:14" /><row r="11" spans="1:14" /><row r="12" spans="1:14" ht="147" customHeight="1" /><row r="13" spans="1:14"><c r="K13" t="s"><v>34</v></c></row><row r="14" spans="1:14" /><row r="15" spans="1:14" ht="13" customHeight="1"><c r="A15" t="s"><v>35</v></c><c r="B15" t="s"><v>36</v></c></row><row r="16" spans="1:14" ht="13" customHeight="1" /><row r="17" spans="1:7"><c r="A17" t="s"><v>37</v></c></row><row r="18" spans="1:7" /><row r="19" spans="1:7" /><row r="20" spans="1:7" /><row r="21" spans="1:7" ht="169.5" customHeight="1" /><row r="22" spans="1:7" /><row r="23" spans="1:7" /><row r="24" spans="1:7" ht="16" customHeight="1"><c r="C24" t="s"><v>38</v></c></row><row r="25" spans="1:7" ht="16" customHeight="1" /><row r="26" spans="1:7" /><row r="27" spans="1:7" /><row r="28" spans="1:7" ht="16" customHeight="1" /><row r="29" spans="1:7" ht="16" customHeight="1"><c r="G29" t="s"><v>39</v></c></row><row r="30" spans="1:7" ht="16" customHeight="1" /><row r="31" spans="1:7" ht="13" customHeight="1" /><row r="49" ht="15.75" customHeight="1" /><row r="50" ht="15.75" customHeight="1" /><row r="51" ht="15.75" customHeight="1" /><row r="52" ht="15.75" customHeight="1" /><row r="53" ht="15.75" customHeight="1" /><row r="54" ht="15.75" customHeight="1" /><row r="55" ht="15.75" customHeight="1" /><row r="56" ht="15.75" customHeight="1" /><row r="57" ht="15.75" customHeight="1" /><row r="58" ht="15.75" customHeight="1" /><row r="59" ht="15.75" customHeight="1" /><row r="60" ht="15.75" customHeight="1" /><row r="61" ht="15.75" customHeight="1" /><row r="62" ht="15.75" customHeight="1" /></sheetData><pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3" /><drawing r:id="rId1" /></worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
working, fix add drawing & update content xml
</commit_message>
<xml_diff>
--- a/excel/output.xlsx
+++ b/excel/output.xlsx
@@ -1232,16 +1232,471 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="UTF-8" standalone="yes"?><xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"><xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main"><xdr:from><xdr:col>11</xdr:col><xdr:colOff>180975</xdr:colOff><xdr:row>29</xdr:row><xdr:rowOff>95250</xdr:rowOff></xdr:from><xdr:ext cx="676275" cy="190500" /><xdr:sp macro="" textlink=""><xdr:nvSpPr><xdr:cNvPr id="3" name="Shape 3"><a:extLst><a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}"><a16:creationId id="{00000000-0008-0000-0100-000003000000}" /></a:ext></a:extLst></xdr:cNvPr><xdr:cNvSpPr /></xdr:nvSpPr><xdr:spPr><a:xfrm><a:off x="16144875" y="9950450" /><a:ext cx="676275" cy="190500" /></a:xfrm><a:prstGeom prst="rect"><a:avLst /></a:prstGeom><a:noFill /><a:ln w="76200" cap="flat" cmpd="sng"><a:solidFill><a:srgbClr val="FF0000" /></a:solidFill><a:prstDash val="solid" /><a:round /><a:headEnd type="none" w="sm" len="sm" /><a:tailEnd type="none" w="sm" len="sm" /></a:ln></xdr:spPr><xdr:txBody><a:bodyPr spcFirstLastPara="1" wrap="square" lIns="91425" tIns="91425" rIns="91425" bIns="91425" anchor="ctr" anchorCtr="0"><a:noAutofit /></a:bodyPr><a:lstStyle /><a:p><a:pPr marL="0" lvl="0" indent="0" algn="ctr" rtl="0"><a:spcBef><a:spcPts val="0" /></a:spcBef><a:spcAft><a:spcPts val="0" /></a:spcAft><a:buNone /></a:pPr><a:endParaRPr sz="1400" /></a:p></xdr:txBody></xdr:sp><xdr:clientData fLocksWithSheet="0" /></xdr:oneCellAnchor><xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main"><xdr:from><xdr:col>4</xdr:col><xdr:colOff>47625</xdr:colOff><xdr:row>25</xdr:row><xdr:rowOff>92074</xdr:rowOff></xdr:from><xdr:ext cx="6734175" cy="796925" /><xdr:grpSp><xdr:nvGrpSpPr><xdr:cNvPr id="2" name="Shape 2" title="Drawing"><a:extLst><a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}"><a16:creationId id="{00000000-0008-0000-0100-000002000000}" /></a:ext></a:extLst></xdr:cNvPr><xdr:cNvGrpSpPr /></xdr:nvGrpSpPr><xdr:grpSpPr><a:xfrm><a:off x="9266331" y="9221133" /><a:ext cx="6734175" cy="796925" /><a:chOff x="2243550" y="4293375" /><a:chExt cx="6030300" cy="89700" /></a:xfrm></xdr:grpSpPr><xdr:cxnSp macro=""><xdr:nvCxnSpPr><xdr:cNvPr id="4" name="Shape 4"><a:extLst><a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}"><a16:creationId id="{00000000-0008-0000-0100-000004000000}" /></a:ext></a:extLst></xdr:cNvPr><xdr:cNvCxnSpPr /></xdr:nvCxnSpPr><xdr:spPr><a:xfrm rot="10800000"><a:off x="2243550" y="4293375" /><a:ext cx="6030300" cy="89700" /></a:xfrm><a:prstGeom prst="straightConnector1"><a:avLst /></a:prstGeom><a:noFill /><a:ln w="28575" cap="flat" cmpd="sng"><a:solidFill><a:srgbClr val="FF0000" /></a:solidFill><a:prstDash val="solid" /><a:round /><a:headEnd type="none" w="med" len="med" /><a:tailEnd type="triangle" w="med" len="med" /></a:ln></xdr:spPr></xdr:cxnSp></xdr:grpSp><xdr:clientData fLocksWithSheet="0" /></xdr:oneCellAnchor><xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main"><xdr:from><xdr:col>0</xdr:col><xdr:colOff>2657475</xdr:colOff><xdr:row>16</xdr:row><xdr:rowOff>200025</xdr:rowOff></xdr:from><xdr:ext cx="2143125" cy="3181350" /><xdr:grpSp><xdr:nvGrpSpPr><xdr:cNvPr id="5" name="Shape 2" title="Drawing"><a:extLst><a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}"><a16:creationId id="{00000000-0008-0000-0100-000005000000}" /></a:ext></a:extLst></xdr:cNvPr><xdr:cNvGrpSpPr /></xdr:nvGrpSpPr><xdr:grpSpPr><a:xfrm><a:off x="2657475" y="5581090" /><a:ext cx="2143125" cy="3181350" /><a:chOff x="3052075" y="2001475" /><a:chExt cx="1841400" cy="2751900" /></a:xfrm></xdr:grpSpPr><xdr:cxnSp macro=""><xdr:nvCxnSpPr><xdr:cNvPr id="6" name="Shape 5"><a:extLst><a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}"><a16:creationId id="{00000000-0008-0000-0100-000006000000}" /></a:ext></a:extLst></xdr:cNvPr><xdr:cNvCxnSpPr /></xdr:nvCxnSpPr><xdr:spPr><a:xfrm rot="10800000"><a:off x="3052075" y="2001475" /><a:ext cx="1841400" cy="2751900" /></a:xfrm><a:prstGeom prst="straightConnector1"><a:avLst /></a:prstGeom><a:noFill /><a:ln w="28575" cap="flat" cmpd="sng"><a:solidFill><a:srgbClr val="FF0000" /></a:solidFill><a:prstDash val="solid" /><a:round /><a:headEnd type="none" w="med" len="med" /><a:tailEnd type="triangle" w="med" len="med" /></a:ln></xdr:spPr></xdr:cxnSp></xdr:grpSp><xdr:clientData fLocksWithSheet="0" /></xdr:oneCellAnchor></xdr:wsDr>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="676275" cy="190500"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Shape 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16144875" y="9950450"/>
+          <a:ext cx="676275" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="76200" cap="flat" cmpd="sng">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="sm" len="sm"/>
+          <a:tailEnd type="none" w="sm" len="sm"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr spcFirstLastPara="1" wrap="square" lIns="91425" tIns="91425" rIns="91425" bIns="91425" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" rtl="0">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>92074</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="6734175" cy="796925"/>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="Shape 2" title="Drawing">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="9266331" y="9221133"/>
+          <a:ext cx="6734175" cy="796925"/>
+          <a:chOff x="2243550" y="4293375"/>
+          <a:chExt cx="6030300" cy="89700"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="4" name="Shape 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId id="{00000000-0008-0000-0100-000004000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="10800000">
+            <a:off x="2243550" y="4293375"/>
+            <a:ext cx="6030300" cy="89700"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="28575" cap="flat" cmpd="sng">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+            <a:headEnd type="none" w="med" len="med"/>
+            <a:tailEnd type="triangle" w="med" len="med"/>
+          </a:ln>
+        </xdr:spPr>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2657475</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2143125" cy="3181350"/>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="5" name="Shape 2" title="Drawing">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2657475" y="5581090"/>
+          <a:ext cx="2143125" cy="3181350"/>
+          <a:chOff x="3052075" y="2001475"/>
+          <a:chExt cx="1841400" cy="2751900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="6" name="Shape 5">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId id="{00000000-0008-0000-0100-000006000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="10800000">
+            <a:off x="3052075" y="2001475"/>
+            <a:ext cx="1841400" cy="2751900"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="28575" cap="flat" cmpd="sng">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+            <a:headEnd type="none" w="med" len="med"/>
+            <a:tailEnd type="triangle" w="med" len="med"/>
+          </a:ln>
+        </xdr:spPr>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="UTF-8" standalone="yes"?><xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"><xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:ns3="http://schemas.openxmlformats.org/officeDocument/2006/relationships"><xdr:from><xdr:col>3</xdr:col><xdr:colOff>0</xdr:colOff><xdr:row>0</xdr:row><xdr:rowOff>0</xdr:rowOff></xdr:from><xdr:ext cx="295275" cy="200025" /><xdr:pic><xdr:nvPicPr><xdr:cNvPr id="2" name="image4.jpg"><a:extLst><a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}"><a16:creationId id="{00000000-0008-0000-0300-000002000000}" /></a:ext></a:extLst></xdr:cNvPr><xdr:cNvPicPr preferRelativeResize="0" /></xdr:nvPicPr><xdr:blipFill><a:blip ns3:embed="rId1" cstate="print" /><a:stretch><a:fillRect /></a:stretch></xdr:blipFill><xdr:spPr><a:prstGeom prst="rect"><a:avLst /></a:prstGeom><a:noFill /></xdr:spPr></xdr:pic><xdr:clientData fLocksWithSheet="0" /></xdr:oneCellAnchor></xdr:wsDr>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:ns3="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="295275" cy="200025"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="image4.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip ns3:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="UTF-8" standalone="yes"?><xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"><xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:ns3="http://schemas.openxmlformats.org/officeDocument/2006/relationships"><xdr:from><xdr:col>4</xdr:col><xdr:colOff>0</xdr:colOff><xdr:row>14</xdr:row><xdr:rowOff>0</xdr:rowOff></xdr:from><xdr:ext cx="8483600" cy="4470400" /><xdr:pic><xdr:nvPicPr><xdr:cNvPr id="5" name="image5.jpg"><a:extLst><a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}"><a16:creationId id="{00000000-0008-0000-0500-000005000000}" /></a:ext></a:extLst></xdr:cNvPr><xdr:cNvPicPr preferRelativeResize="0" /></xdr:nvPicPr><xdr:blipFill><a:blip ns3:embed="rId1" cstate="print" /><a:stretch><a:fillRect /></a:stretch></xdr:blipFill><xdr:spPr><a:xfrm><a:off x="9271000" y="5829300" /><a:ext cx="8483600" cy="4470400" /></a:xfrm><a:prstGeom prst="rect"><a:avLst /></a:prstGeom><a:noFill /></xdr:spPr></xdr:pic><xdr:clientData fLocksWithSheet="0" /></xdr:oneCellAnchor><xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main"><xdr:from><xdr:col>3</xdr:col><xdr:colOff>933450</xdr:colOff><xdr:row>27</xdr:row><xdr:rowOff>38100</xdr:rowOff></xdr:from><xdr:ext cx="6496050" cy="152400" /><xdr:grpSp><xdr:nvGrpSpPr><xdr:cNvPr id="2" name="Shape 2" title="Drawing"><a:extLst><a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}"><a16:creationId id="{00000000-0008-0000-0500-000002000000}" /></a:ext></a:extLst></xdr:cNvPr><xdr:cNvGrpSpPr /></xdr:nvGrpSpPr><xdr:grpSpPr><a:xfrm><a:off x="9239250" y="9893300" /><a:ext cx="6496050" cy="152400" /><a:chOff x="2243550" y="4293375" /><a:chExt cx="6030300" cy="89700" /></a:xfrm></xdr:grpSpPr><xdr:cxnSp macro=""><xdr:nvCxnSpPr><xdr:cNvPr id="6" name="Shape 6"><a:extLst><a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}"><a16:creationId id="{00000000-0008-0000-0500-000006000000}" /></a:ext></a:extLst></xdr:cNvPr><xdr:cNvCxnSpPr /></xdr:nvCxnSpPr><xdr:spPr><a:xfrm rot="10800000"><a:off x="2243550" y="4293375" /><a:ext cx="6030300" cy="89700" /></a:xfrm><a:prstGeom prst="straightConnector1"><a:avLst /></a:prstGeom><a:noFill /><a:ln w="28575" cap="flat" cmpd="sng"><a:solidFill><a:srgbClr val="FF0000" /></a:solidFill><a:prstDash val="solid" /><a:round /><a:headEnd type="none" w="med" len="med" /><a:tailEnd type="triangle" w="med" len="med" /></a:ln></xdr:spPr></xdr:cxnSp></xdr:grpSp><xdr:clientData fLocksWithSheet="0" /></xdr:oneCellAnchor><xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main"><xdr:from><xdr:col>0</xdr:col><xdr:colOff>819150</xdr:colOff><xdr:row>17</xdr:row><xdr:rowOff>161925</xdr:rowOff></xdr:from><xdr:ext cx="2143125" cy="3190875" /><xdr:grpSp><xdr:nvGrpSpPr><xdr:cNvPr id="3" name="Shape 2" title="Drawing"><a:extLst><a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}"><a16:creationId id="{00000000-0008-0000-0500-000003000000}" /></a:ext></a:extLst></xdr:cNvPr><xdr:cNvGrpSpPr /></xdr:nvGrpSpPr><xdr:grpSpPr><a:xfrm><a:off x="819150" y="6511925" /><a:ext cx="2143125" cy="3190875" /><a:chOff x="3052075" y="2001475" /><a:chExt cx="1841400" cy="2751900" /></a:xfrm></xdr:grpSpPr><xdr:cxnSp macro=""><xdr:nvCxnSpPr><xdr:cNvPr id="7" name="Shape 7"><a:extLst><a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}"><a16:creationId id="{00000000-0008-0000-0500-000007000000}" /></a:ext></a:extLst></xdr:cNvPr><xdr:cNvCxnSpPr /></xdr:nvCxnSpPr><xdr:spPr><a:xfrm rot="10800000"><a:off x="3052075" y="2001475" /><a:ext cx="1841400" cy="2751900" /></a:xfrm><a:prstGeom prst="straightConnector1"><a:avLst /></a:prstGeom><a:noFill /><a:ln w="28575" cap="flat" cmpd="sng"><a:solidFill><a:srgbClr val="FF0000" /></a:solidFill><a:prstDash val="solid" /><a:round /><a:headEnd type="none" w="med" len="med" /><a:tailEnd type="triangle" w="med" len="med" /></a:ln></xdr:spPr></xdr:cxnSp></xdr:grpSp><xdr:clientData fLocksWithSheet="0" /></xdr:oneCellAnchor><xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:ns3="http://schemas.openxmlformats.org/officeDocument/2006/relationships"><xdr:from><xdr:col>4</xdr:col><xdr:colOff>0</xdr:colOff><xdr:row>2</xdr:row><xdr:rowOff>0</xdr:rowOff></xdr:from><xdr:ext cx="8724900" cy="5016500" /><xdr:pic><xdr:nvPicPr><xdr:cNvPr id="4" name="image6.jpg"><a:extLst><a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}"><a16:creationId id="{00000000-0008-0000-0500-000004000000}" /></a:ext></a:extLst></xdr:cNvPr><xdr:cNvPicPr preferRelativeResize="0" /></xdr:nvPicPr><xdr:blipFill><a:blip ns3:embed="rId2" cstate="print" /><a:stretch><a:fillRect /></a:stretch></xdr:blipFill><xdr:spPr><a:xfrm><a:off x="9271000" y="381000" /><a:ext cx="8724900" cy="5016500" /></a:xfrm><a:prstGeom prst="rect"><a:avLst /></a:prstGeom><a:noFill /></xdr:spPr></xdr:pic><xdr:clientData fLocksWithSheet="0" /></xdr:oneCellAnchor></xdr:wsDr>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:ns3="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="8483600" cy="4470400"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="image5.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId id="{00000000-0008-0000-0500-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip ns3:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9271000" y="5829300"/>
+          <a:ext cx="8483600" cy="4470400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>933450</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="6496050" cy="152400"/>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="Shape 2" title="Drawing">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId id="{00000000-0008-0000-0500-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="9239250" y="9893300"/>
+          <a:ext cx="6496050" cy="152400"/>
+          <a:chOff x="2243550" y="4293375"/>
+          <a:chExt cx="6030300" cy="89700"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="6" name="Shape 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId id="{00000000-0008-0000-0500-000006000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="10800000">
+            <a:off x="2243550" y="4293375"/>
+            <a:ext cx="6030300" cy="89700"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="28575" cap="flat" cmpd="sng">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+            <a:headEnd type="none" w="med" len="med"/>
+            <a:tailEnd type="triangle" w="med" len="med"/>
+          </a:ln>
+        </xdr:spPr>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2143125" cy="3190875"/>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="3" name="Shape 2" title="Drawing">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId id="{00000000-0008-0000-0500-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="819150" y="6511925"/>
+          <a:ext cx="2143125" cy="3190875"/>
+          <a:chOff x="3052075" y="2001475"/>
+          <a:chExt cx="1841400" cy="2751900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="7" name="Shape 7">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId id="{00000000-0008-0000-0500-000007000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="10800000">
+            <a:off x="3052075" y="2001475"/>
+            <a:ext cx="1841400" cy="2751900"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="28575" cap="flat" cmpd="sng">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+            <a:headEnd type="none" w="med" len="med"/>
+            <a:tailEnd type="triangle" w="med" len="med"/>
+          </a:ln>
+        </xdr:spPr>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:ns3="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="8724900" cy="5016500"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="image6.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId id="{00000000-0008-0000-0500-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip ns3:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9271000" y="381000"/>
+          <a:ext cx="8724900" cy="5016500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="UTF-8" standalone="yes"?><xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"><xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:ns3="http://schemas.openxmlformats.org/officeDocument/2006/relationships"><xdr:from><xdr:col>3</xdr:col><xdr:colOff>0</xdr:colOff><xdr:row>0</xdr:row><xdr:rowOff>0</xdr:rowOff></xdr:from><xdr:ext cx="295275" cy="200025" /><xdr:pic><xdr:nvPicPr><xdr:cNvPr id="2" name="image3.jpg"><a:extLst><a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}"><a16:creationId id="{00000000-0008-0000-0700-000002000000}" /></a:ext></a:extLst></xdr:cNvPr><xdr:cNvPicPr preferRelativeResize="0" /></xdr:nvPicPr><xdr:blipFill><a:blip ns3:embed="rId1" cstate="print" /><a:stretch><a:fillRect /></a:stretch></xdr:blipFill><xdr:spPr><a:prstGeom prst="rect"><a:avLst /></a:prstGeom><a:noFill /></xdr:spPr></xdr:pic><xdr:clientData fLocksWithSheet="0" /></xdr:oneCellAnchor></xdr:wsDr>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:ns3="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="295275" cy="200025"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="image3.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId id="{00000000-0008-0000-0700-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip ns3:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1682,8 +2137,109 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version='1.0' encoding='UTF-8'?>
-<worksheet><dimension ref="A3:N62" /><sheetViews><sheetView workbookViewId="0" /></sheetViews><sheetFormatPr defaultRowHeight="15" /><cols><col min="1" max="1" width="40.42578125" customWidth="1" /><col min="2" max="2" width="10.85546875" customWidth="1" /><col min="3" max="3" width="59" customWidth="1" /><col min="13" max="13" width="6.42578125" customWidth="1" /></cols><sheetData><row r="3" spans="1:14" ht="13" customHeight="1"><c r="N3" t="s"><v>29</v></c></row><row r="4" spans="1:14" ht="13" customHeight="1" /><row r="5" spans="1:14" ht="13" customHeight="1" /><row r="6" spans="1:14" ht="13" customHeight="1"><c r="A6" t="s"><v>30</v></c><c r="B6" t="s"><v>31</v></c></row><row r="7" spans="1:14" ht="13" customHeight="1" /><row r="8" spans="1:14" ht="50.25" customHeight="1"><c r="A8" t="s"><v>32</v></c></row><row r="9" spans="1:14" ht="45" customHeight="1"><c r="A9" t="s"><v>33</v></c></row><row r="10" spans="1:14" /><row r="11" spans="1:14" /><row r="12" spans="1:14" ht="147" customHeight="1" /><row r="13" spans="1:14"><c r="K13" t="s"><v>34</v></c></row><row r="14" spans="1:14" /><row r="15" spans="1:14" ht="13" customHeight="1"><c r="A15" t="s"><v>35</v></c><c r="B15" t="s"><v>36</v></c></row><row r="16" spans="1:14" ht="13" customHeight="1" /><row r="17" spans="1:7"><c r="A17" t="s"><v>37</v></c></row><row r="18" spans="1:7" /><row r="19" spans="1:7" /><row r="20" spans="1:7" /><row r="21" spans="1:7" ht="169.5" customHeight="1" /><row r="22" spans="1:7" /><row r="23" spans="1:7" /><row r="24" spans="1:7" ht="16" customHeight="1"><c r="C24" t="s"><v>38</v></c></row><row r="25" spans="1:7" ht="16" customHeight="1" /><row r="26" spans="1:7" /><row r="27" spans="1:7" /><row r="28" spans="1:7" ht="16" customHeight="1" /><row r="29" spans="1:7" ht="16" customHeight="1"><c r="G29" t="s"><v>39</v></c></row><row r="30" spans="1:7" ht="16" customHeight="1" /><row r="31" spans="1:7" ht="13" customHeight="1" /><row r="49" ht="15.75" customHeight="1" /><row r="50" ht="15.75" customHeight="1" /><row r="51" ht="15.75" customHeight="1" /><row r="52" ht="15.75" customHeight="1" /><row r="53" ht="15.75" customHeight="1" /><row r="54" ht="15.75" customHeight="1" /><row r="55" ht="15.75" customHeight="1" /><row r="56" ht="15.75" customHeight="1" /><row r="57" ht="15.75" customHeight="1" /><row r="58" ht="15.75" customHeight="1" /><row r="59" ht="15.75" customHeight="1" /><row r="60" ht="15.75" customHeight="1" /><row r="61" ht="15.75" customHeight="1" /><row r="62" ht="15.75" customHeight="1" /></sheetData><pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3" /><drawing r:id="rId1" /></worksheet>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A3:N62"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="40.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="59" customWidth="1"/>
+    <col min="13" max="13" width="6.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:14" ht="13" customHeight="1">
+      <c r="N3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="13" customHeight="1"/>
+    <row r="5" spans="1:14" ht="13" customHeight="1"/>
+    <row r="6" spans="1:14" ht="13" customHeight="1">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="13" customHeight="1"/>
+    <row r="8" spans="1:14" ht="50.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="45" customHeight="1">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14"/>
+    <row r="11" spans="1:14"/>
+    <row r="12" spans="1:14" ht="147" customHeight="1"/>
+    <row r="13" spans="1:14">
+      <c r="K13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14"/>
+    <row r="15" spans="1:14" ht="13" customHeight="1">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="13" customHeight="1"/>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7"/>
+    <row r="19" spans="1:7"/>
+    <row r="20" spans="1:7"/>
+    <row r="21" spans="1:7" ht="169.5" customHeight="1"/>
+    <row r="22" spans="1:7"/>
+    <row r="23" spans="1:7"/>
+    <row r="24" spans="1:7" ht="16" customHeight="1">
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="16" customHeight="1"/>
+    <row r="26" spans="1:7"/>
+    <row r="27" spans="1:7"/>
+    <row r="28" spans="1:7" ht="16" customHeight="1"/>
+    <row r="29" spans="1:7" ht="16" customHeight="1">
+      <c r="G29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="16" customHeight="1"/>
+    <row r="31" spans="1:7" ht="13" customHeight="1"/>
+    <row r="49" ht="15.75" customHeight="1"/>
+    <row r="50" ht="15.75" customHeight="1"/>
+    <row r="51" ht="15.75" customHeight="1"/>
+    <row r="52" ht="15.75" customHeight="1"/>
+    <row r="53" ht="15.75" customHeight="1"/>
+    <row r="54" ht="15.75" customHeight="1"/>
+    <row r="55" ht="15.75" customHeight="1"/>
+    <row r="56" ht="15.75" customHeight="1"/>
+    <row r="57" ht="15.75" customHeight="1"/>
+    <row r="58" ht="15.75" customHeight="1"/>
+    <row r="59" ht="15.75" customHeight="1"/>
+    <row r="60" ht="15.75" customHeight="1"/>
+    <row r="61" ht="15.75" customHeight="1"/>
+    <row r="62" ht="15.75" customHeight="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4675,6 +5231,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4937,6 +5494,7 @@
     <row r="34" ht="13" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7808,5 +8366,6 @@
     <row r="24" spans="2:5" ht="13" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>